<commit_message>
add a false case
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaofan03/Documents/ks/api_auto_test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B45BF-61CE-3F4F-9A6B-710760E6BD05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E932DC8-8023-7C4C-A3AF-263DF3482557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7080" yWindow="-25500" windowWidth="28800" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>2016-10-10</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>2018</t>
+  </si>
+  <si>
+    <t>False</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -490,7 +502,15 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="C8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>